<commit_message>
Secdep Loan, Saving, RD scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/4767-SUBMITRD01JAN2015(AMT5000-PRD06MNTHwithINCT-1)-APRACT01JAN2015.xlsx
+++ b/Finflux Automation Excels/Client/4767-SUBMITRD01JAN2015(AMT5000-PRD06MNTHwithINCT-1)-APRACT01JAN2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>